<commit_message>
Italian scenario text edited
</commit_message>
<xml_diff>
--- a/stm-unity/Assets/Resources/Localization/Sports Team Manager Scenario Localization.xlsx
+++ b/stm-unity/Assets/Resources/Localization/Sports Team Manager Scenario Localization.xlsx
@@ -381,10 +381,10 @@
     <t>PWAvoidingCollaboratingCollaborating</t>
   </si>
   <si>
-    <t>OK, we'll take half an hour to talk about it after the next session.</t>
-  </si>
-  <si>
-    <t>Dai che domani ci prendiamo mezz'ora.</t>
+    <t>OK, we'll take half an hour to talk about it as soon as possible.</t>
+  </si>
+  <si>
+    <t>Ci prendiamo mezz'ora il prima possibile.</t>
   </si>
   <si>
     <t>PWAvoidingCollaboratingAvoiding</t>
@@ -1020,7 +1020,7 @@
     <t>You're always right...</t>
   </si>
   <si>
-    <t>Hai sempre ragione tu.</t>
+    <t>Hai sempre ragione tu!</t>
   </si>
   <si>
     <t>NotPickedNP21</t>
@@ -1107,7 +1107,7 @@
     <t>Before the next race, we'll take a bit of time to analyze the issue.</t>
   </si>
   <si>
-    <t>Ti va bene se mercoledì dopo l'allenamento ci prendiamo un po’ di tempo per analizzare la questione.</t>
+    <t>Ti va bene se dopo l'allenamento ci prendiamo un po’ di tempo per analizzare la questione.</t>
   </si>
   <si>
     <t>NotPickedAccommodatingCollaboratingAccommodating</t>
@@ -3322,7 +3322,7 @@
       <c r="B27" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="C27" s="2" t="s">
+      <c r="C27" s="1" t="s">
         <v>78</v>
       </c>
     </row>
@@ -9122,7 +9122,7 @@
       <c r="B31" s="11" t="s">
         <v>318</v>
       </c>
-      <c r="C31" s="11" t="s">
+      <c r="C31" s="9" t="s">
         <v>319</v>
       </c>
     </row>

</xml_diff>